<commit_message>
finalized text for multivariate model
</commit_message>
<xml_diff>
--- a/docs/dcc_garch.xlsx
+++ b/docs/dcc_garch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vladimir\Desktop\FMFI_1\Магистерские курсы\Эконометрика\Прочие материалы\HW2\metrics_HW2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A1FD76-6530-4694-9927-4B10DBF1B378}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED3CDB5-77EE-49C7-9F40-94D309DC1CCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,8 +148,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -228,22 +228,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -252,7 +252,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -34164,8 +34164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F987"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>